<commit_message>
Add LI.xlsx to excel-files
</commit_message>
<xml_diff>
--- a/excel-files/naming-service/BO-BEND-FAMS.xlsx
+++ b/excel-files/naming-service/BO-BEND-FAMS.xlsx
@@ -47,7 +47,7 @@
     <t>PS</t>
   </si>
   <si>
-    <t>DIPB</t>
+    <t>B</t>
   </si>
   <si>
     <t>Fam2</t>
@@ -140,15 +140,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -172,64 +172,62 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.83333333333333"/>
-    <col collapsed="false" hidden="false" max="7" min="2" style="1" width="8.83333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.83333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>